<commit_message>
Changes in LocationsService, initial implementation of more advanced error handling, minor improvements.
</commit_message>
<xml_diff>
--- a/openrouteservice/docs/services/locations/POICategories.xlsx
+++ b/openrouteservice/docs/services/locations/POICategories.xlsx
@@ -305,9 +305,6 @@
     <t>guest_house</t>
   </si>
   <si>
-    <t>apparmtent</t>
-  </si>
-  <si>
     <t>hostel</t>
   </si>
   <si>
@@ -971,9 +968,6 @@
     <t>#arts_and_culture</t>
   </si>
   <si>
-    <t>#leisure_and_ntertainment</t>
-  </si>
-  <si>
     <t>#financial</t>
   </si>
   <si>
@@ -1089,6 +1083,12 @@
   </si>
   <si>
     <t>coworking_space</t>
+  </si>
+  <si>
+    <t>#leisure_and_entertainment</t>
+  </si>
+  <si>
+    <t>appartment</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1096,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1192,7 +1192,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1495,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
-      <selection activeCell="F330" sqref="F330"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1507,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C1" s="1">
         <v>100</v>
@@ -1530,7 +1530,7 @@
         <v>87</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>93</v>
+        <v>354</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C11" si="0">C2+1</f>
@@ -1590,7 +1590,7 @@
         <v>87</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -1602,7 +1602,7 @@
         <v>87</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -1614,7 +1614,7 @@
         <v>87</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -1626,7 +1626,7 @@
         <v>87</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C14" s="1">
         <v>120</v>
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C15">
         <f>C14+1</f>
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:C18" si="1">C15+1</f>
@@ -1682,7 +1682,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="1">
@@ -1711,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C22">
         <f>C21+1</f>
@@ -1723,7 +1723,7 @@
         <v>87</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C23">
         <f t="shared" ref="C23:C27" si="2">C22+1</f>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C24">
         <f t="shared" si="2"/>
@@ -1747,7 +1747,7 @@
         <v>87</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
@@ -1759,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C30" s="1">
         <v>150</v>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C31" s="4">
         <f>C30+1</f>
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" ref="C32:C37" si="3">C31+1</f>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="3"/>
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="3"/>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="3"/>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="3"/>
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="3"/>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="39" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C39" s="1">
         <v>160</v>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C40" s="4">
         <f>C39+1</f>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" ref="C41:C61" si="4">C40+1</f>
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="4"/>
@@ -1937,10 +1937,10 @@
     </row>
     <row r="44" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="4"/>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="4"/>
@@ -1976,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="4"/>
@@ -1988,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="4"/>
@@ -2000,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C49" s="4">
         <f t="shared" si="4"/>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C50" s="4">
         <f t="shared" si="4"/>
@@ -2024,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C51" s="4">
         <f t="shared" si="4"/>
@@ -2036,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C52" s="4">
         <f t="shared" si="4"/>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" si="4"/>
@@ -2060,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" si="4"/>
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C55" s="4">
         <f t="shared" si="4"/>
@@ -2084,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C56" s="4">
         <f t="shared" si="4"/>
@@ -2096,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C57" s="4">
         <f t="shared" si="4"/>
@@ -2108,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="4"/>
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="4">
         <f t="shared" si="4"/>
@@ -2132,7 +2132,7 @@
         <v>0</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C60" s="4">
         <f t="shared" si="4"/>
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C61" s="4">
         <f t="shared" si="4"/>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="64" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C64" s="1">
         <v>190</v>
@@ -2172,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C65" s="4">
         <f>C64+1</f>
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C66" s="4">
         <f t="shared" ref="C66:C67" si="5">C65+1</f>
@@ -2196,7 +2196,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C67" s="4">
         <f t="shared" si="5"/>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C70" s="1">
         <v>200</v>
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C75" s="4">
         <f t="shared" si="6"/>
@@ -2316,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C79" s="4">
         <f t="shared" si="6"/>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="84" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C84" s="1">
         <v>220</v>
@@ -2363,10 +2363,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C85" s="4">
         <f>C84+1</f>
@@ -2375,10 +2375,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B86" s="9" t="s">
         <v>317</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>319</v>
       </c>
       <c r="C86" s="4">
         <f t="shared" ref="C86:C113" si="7">C85+1</f>
@@ -2387,10 +2387,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C87" s="4">
         <f t="shared" si="7"/>
@@ -2399,10 +2399,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C88" s="4">
         <f t="shared" si="7"/>
@@ -2411,10 +2411,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C89" s="4">
         <f t="shared" si="7"/>
@@ -2423,10 +2423,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C90" s="4">
         <f t="shared" si="7"/>
@@ -2435,10 +2435,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C91" s="4">
         <f t="shared" si="7"/>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C92" s="4">
         <f t="shared" si="7"/>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C93" s="4">
         <f t="shared" si="7"/>
@@ -2471,10 +2471,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C94" s="4">
         <f t="shared" si="7"/>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>46</v>
@@ -2495,10 +2495,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C96" s="4">
         <f t="shared" si="7"/>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C97" s="4">
         <f t="shared" si="7"/>
@@ -2519,10 +2519,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C98" s="4">
         <f t="shared" si="7"/>
@@ -2531,10 +2531,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C99" s="4">
         <f t="shared" si="7"/>
@@ -2543,10 +2543,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C100" s="4">
         <f t="shared" si="7"/>
@@ -2555,10 +2555,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C101" s="4">
         <f t="shared" si="7"/>
@@ -2567,10 +2567,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C102" s="4">
         <f t="shared" si="7"/>
@@ -2579,10 +2579,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C103" s="4">
         <f t="shared" si="7"/>
@@ -2591,10 +2591,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C104" s="4">
         <f t="shared" si="7"/>
@@ -2603,10 +2603,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C105" s="4">
         <f t="shared" si="7"/>
@@ -2615,10 +2615,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C106" s="4">
         <f t="shared" si="7"/>
@@ -2627,10 +2627,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C107" s="4">
         <f t="shared" si="7"/>
@@ -2639,10 +2639,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C108" s="4">
         <f t="shared" si="7"/>
@@ -2651,10 +2651,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C109" s="4">
         <f t="shared" si="7"/>
@@ -2663,10 +2663,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C110" s="4">
         <f t="shared" si="7"/>
@@ -2675,10 +2675,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C111" s="4">
         <f t="shared" si="7"/>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C112" s="4">
         <f t="shared" si="7"/>
@@ -2699,10 +2699,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C113" s="4">
         <f t="shared" si="7"/>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="116" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>315</v>
+        <v>353</v>
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="1">
@@ -2723,10 +2723,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B117" s="7" t="s">
         <v>263</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>264</v>
       </c>
       <c r="C117">
         <f>C116+1</f>
@@ -2735,10 +2735,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C118">
         <f t="shared" ref="C118:C166" si="8">C117+1</f>
@@ -2747,10 +2747,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C119">
         <f t="shared" si="8"/>
@@ -2759,10 +2759,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C120">
         <f t="shared" si="8"/>
@@ -2771,10 +2771,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C121">
         <f t="shared" si="8"/>
@@ -2783,10 +2783,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C122">
         <f t="shared" si="8"/>
@@ -2795,10 +2795,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C123">
         <f t="shared" si="8"/>
@@ -2807,10 +2807,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C124">
         <f t="shared" si="8"/>
@@ -2819,10 +2819,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C125">
         <f>C124+1</f>
@@ -2831,7 +2831,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B126" s="7" t="s">
         <v>54</v>
@@ -2843,10 +2843,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C127">
         <f t="shared" si="8"/>
@@ -2855,10 +2855,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C128">
         <f t="shared" si="8"/>
@@ -2867,10 +2867,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C129">
         <f t="shared" si="8"/>
@@ -2879,10 +2879,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C130">
         <f t="shared" si="8"/>
@@ -2891,10 +2891,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C131">
         <f t="shared" si="8"/>
@@ -2903,10 +2903,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C132">
         <f t="shared" si="8"/>
@@ -2915,10 +2915,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C133">
         <f t="shared" si="8"/>
@@ -2927,10 +2927,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C134">
         <f t="shared" si="8"/>
@@ -2939,10 +2939,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C135">
         <f t="shared" si="8"/>
@@ -2951,10 +2951,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C136">
         <f t="shared" si="8"/>
@@ -2963,10 +2963,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C137">
         <f t="shared" si="8"/>
@@ -2975,10 +2975,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C138">
         <f t="shared" si="8"/>
@@ -2987,10 +2987,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C139">
         <f t="shared" si="8"/>
@@ -2999,10 +2999,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C140">
         <f t="shared" si="8"/>
@@ -3011,10 +3011,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C141">
         <f t="shared" si="8"/>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B142" s="7" t="s">
         <v>75</v>
@@ -3035,10 +3035,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C143">
         <f t="shared" si="8"/>
@@ -3047,10 +3047,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C144">
         <f t="shared" si="8"/>
@@ -3059,10 +3059,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C145">
         <f t="shared" si="8"/>
@@ -3071,10 +3071,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C146">
         <f t="shared" si="8"/>
@@ -3083,10 +3083,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C147">
         <f t="shared" si="8"/>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B148" s="7" t="s">
         <v>86</v>
@@ -3107,10 +3107,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C149">
         <f t="shared" si="8"/>
@@ -3119,10 +3119,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C150">
         <f t="shared" si="8"/>
@@ -3131,10 +3131,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C151">
         <f t="shared" si="8"/>
@@ -3143,10 +3143,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C152">
         <f t="shared" si="8"/>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C153">
         <f t="shared" si="8"/>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C154">
         <f t="shared" si="8"/>
@@ -3182,7 +3182,7 @@
         <v>0</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C155">
         <f t="shared" si="8"/>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C156">
         <f t="shared" si="8"/>
@@ -3206,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C157">
         <f t="shared" si="8"/>
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C158">
         <f t="shared" si="8"/>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C160">
         <f t="shared" si="8"/>
@@ -3254,7 +3254,7 @@
         <v>0</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C161">
         <f t="shared" si="8"/>
@@ -3266,7 +3266,7 @@
         <v>0</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C162">
         <f t="shared" si="8"/>
@@ -3290,7 +3290,7 @@
         <v>87</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C164">
         <f t="shared" si="8"/>
@@ -3302,7 +3302,7 @@
         <v>87</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C165">
         <f t="shared" si="8"/>
@@ -3314,7 +3314,7 @@
         <v>87</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C166">
         <f t="shared" si="8"/>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="169" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C169" s="1">
         <v>330</v>
@@ -3335,10 +3335,10 @@
     </row>
     <row r="170" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C170">
         <f>C169+1</f>
@@ -3347,10 +3347,10 @@
     </row>
     <row r="171" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C171">
         <f t="shared" ref="C171:C179" si="9">C170+1</f>
@@ -3359,10 +3359,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C172">
         <f t="shared" si="9"/>
@@ -3371,10 +3371,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C173">
         <f t="shared" si="9"/>
@@ -3383,10 +3383,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C174">
         <f t="shared" si="9"/>
@@ -3395,10 +3395,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C175">
         <f t="shared" si="9"/>
@@ -3407,10 +3407,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C176">
         <f t="shared" si="9"/>
@@ -3419,10 +3419,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C177">
         <f t="shared" si="9"/>
@@ -3431,10 +3431,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C178">
         <f t="shared" si="9"/>
@@ -3443,10 +3443,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C179">
         <f t="shared" si="9"/>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="182" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C182" s="1">
         <v>360</v>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C183" s="4">
         <f>C182+1</f>
@@ -3481,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C184" s="4">
         <f t="shared" ref="C184:C196" si="10">C183+1</f>
@@ -3493,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C185" s="4">
         <f t="shared" si="10"/>
@@ -3505,7 +3505,7 @@
         <v>0</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C186" s="4">
         <f t="shared" si="10"/>
@@ -3517,7 +3517,7 @@
         <v>0</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C187" s="4">
         <f t="shared" si="10"/>
@@ -3529,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C188" s="4">
         <f t="shared" si="10"/>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C189" s="4">
         <f t="shared" si="10"/>
@@ -3553,7 +3553,7 @@
         <v>0</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C190" s="4">
         <f t="shared" si="10"/>
@@ -3565,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C191" s="4">
         <f t="shared" si="10"/>
@@ -3577,7 +3577,7 @@
         <v>0</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C192" s="4">
         <f t="shared" si="10"/>
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C193" s="4">
         <f t="shared" si="10"/>
@@ -3601,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C194" s="4">
         <f t="shared" si="10"/>
@@ -3613,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C195" s="4">
         <f t="shared" si="10"/>
@@ -3625,7 +3625,7 @@
         <v>0</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C196" s="4">
         <f t="shared" si="10"/>
@@ -3635,7 +3635,7 @@
     <row r="197" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="199" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C199" s="1">
         <v>390</v>
@@ -3658,7 +3658,7 @@
         <v>11</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C201" s="4">
         <f t="shared" ref="C201:C209" si="11">C200+1</f>
@@ -3670,7 +3670,7 @@
         <v>11</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C202" s="4">
         <f t="shared" si="11"/>
@@ -3683,7 +3683,7 @@
         <v>11</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C203" s="4">
         <f t="shared" si="11"/>
@@ -3708,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C205" s="4">
         <f t="shared" si="11"/>
@@ -3733,7 +3733,7 @@
         <v>0</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C207" s="4">
         <f t="shared" si="11"/>
@@ -3746,7 +3746,7 @@
         <v>11</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C208" s="4">
         <f t="shared" si="11"/>
@@ -3758,7 +3758,7 @@
         <v>11</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C209" s="4">
         <f t="shared" si="11"/>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="212" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B212" s="6"/>
       <c r="C212" s="1">
@@ -3782,7 +3782,7 @@
         <v>11</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C213">
         <f>C212+1</f>
@@ -3854,7 +3854,7 @@
         <v>11</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C219">
         <f t="shared" si="12"/>
@@ -3962,7 +3962,7 @@
         <v>11</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C228">
         <f t="shared" si="12"/>
@@ -3974,7 +3974,7 @@
         <v>11</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C229">
         <f t="shared" si="12"/>
@@ -4010,7 +4010,7 @@
         <v>11</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C232">
         <f t="shared" si="12"/>
@@ -4022,7 +4022,7 @@
         <v>11</v>
       </c>
       <c r="B233" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C233">
         <f t="shared" si="12"/>
@@ -4226,7 +4226,7 @@
         <v>11</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C250">
         <f t="shared" si="12"/>
@@ -4262,7 +4262,7 @@
         <v>11</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C253">
         <f t="shared" si="12"/>
@@ -4346,7 +4346,7 @@
         <v>11</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C260">
         <f t="shared" si="12"/>
@@ -4370,7 +4370,7 @@
         <v>11</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C262">
         <f t="shared" si="12"/>
@@ -4382,7 +4382,7 @@
         <v>11</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C263">
         <f t="shared" si="12"/>
@@ -4442,7 +4442,7 @@
         <v>11</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C268">
         <f t="shared" si="12"/>
@@ -4514,7 +4514,7 @@
         <v>11</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C274">
         <f t="shared" si="12"/>
@@ -4526,7 +4526,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C275">
         <f t="shared" si="12"/>
@@ -4545,7 +4545,7 @@
         <v>484</v>
       </c>
       <c r="F276" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
@@ -4565,7 +4565,7 @@
         <v>11</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C278">
         <f t="shared" ref="C278:C325" si="13">C277+1</f>
@@ -4577,7 +4577,7 @@
         <v>11</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C279">
         <f t="shared" si="13"/>
@@ -4613,7 +4613,7 @@
         <v>11</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C282">
         <f t="shared" si="13"/>
@@ -4625,7 +4625,7 @@
         <v>11</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C283">
         <f t="shared" si="13"/>
@@ -4637,7 +4637,7 @@
         <v>11</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C284">
         <f t="shared" si="13"/>
@@ -4661,7 +4661,7 @@
         <v>11</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C286">
         <f t="shared" si="13"/>
@@ -4685,7 +4685,7 @@
         <v>11</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C288">
         <f t="shared" si="13"/>
@@ -4709,7 +4709,7 @@
         <v>11</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C290">
         <f t="shared" si="13"/>
@@ -4721,7 +4721,7 @@
         <v>11</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C291">
         <f t="shared" si="13"/>
@@ -4757,7 +4757,7 @@
         <v>11</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C294">
         <f t="shared" si="13"/>
@@ -4769,7 +4769,7 @@
         <v>11</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C295">
         <f t="shared" si="13"/>
@@ -4781,7 +4781,7 @@
         <v>11</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C296">
         <f t="shared" si="13"/>
@@ -4793,7 +4793,7 @@
         <v>11</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C297">
         <f t="shared" si="13"/>
@@ -4805,7 +4805,7 @@
         <v>11</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C298">
         <f t="shared" si="13"/>
@@ -4817,7 +4817,7 @@
         <v>11</v>
       </c>
       <c r="B299" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C299">
         <f t="shared" si="13"/>
@@ -4829,7 +4829,7 @@
         <v>11</v>
       </c>
       <c r="B300" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C300">
         <f t="shared" si="13"/>
@@ -4841,7 +4841,7 @@
         <v>11</v>
       </c>
       <c r="B301" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C301">
         <f t="shared" si="13"/>
@@ -4853,7 +4853,7 @@
         <v>11</v>
       </c>
       <c r="B302" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C302">
         <f t="shared" si="13"/>
@@ -4865,7 +4865,7 @@
         <v>11</v>
       </c>
       <c r="B303" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C303">
         <f t="shared" si="13"/>
@@ -4877,7 +4877,7 @@
         <v>11</v>
       </c>
       <c r="B304" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C304">
         <f t="shared" si="13"/>
@@ -4889,7 +4889,7 @@
         <v>11</v>
       </c>
       <c r="B305" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C305">
         <f t="shared" si="13"/>
@@ -4901,7 +4901,7 @@
         <v>11</v>
       </c>
       <c r="B306" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C306">
         <f t="shared" si="13"/>
@@ -4913,7 +4913,7 @@
         <v>11</v>
       </c>
       <c r="B307" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C307">
         <f t="shared" si="13"/>
@@ -4925,7 +4925,7 @@
         <v>11</v>
       </c>
       <c r="B308" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C308">
         <f t="shared" si="13"/>
@@ -4937,7 +4937,7 @@
         <v>11</v>
       </c>
       <c r="B309" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C309">
         <f t="shared" si="13"/>
@@ -4949,7 +4949,7 @@
         <v>11</v>
       </c>
       <c r="B310" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C310">
         <f t="shared" si="13"/>
@@ -4973,7 +4973,7 @@
         <v>11</v>
       </c>
       <c r="B312" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C312">
         <f t="shared" si="13"/>
@@ -4985,7 +4985,7 @@
         <v>11</v>
       </c>
       <c r="B313" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C313">
         <f t="shared" si="13"/>
@@ -4997,7 +4997,7 @@
         <v>11</v>
       </c>
       <c r="B314" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C314">
         <f t="shared" si="13"/>
@@ -5009,7 +5009,7 @@
         <v>11</v>
       </c>
       <c r="B315" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C315">
         <f t="shared" si="13"/>
@@ -5021,7 +5021,7 @@
         <v>11</v>
       </c>
       <c r="B316" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C316">
         <f t="shared" si="13"/>
@@ -5033,7 +5033,7 @@
         <v>11</v>
       </c>
       <c r="B317" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C317">
         <f t="shared" si="13"/>
@@ -5045,7 +5045,7 @@
         <v>11</v>
       </c>
       <c r="B318" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C318">
         <f t="shared" si="13"/>
@@ -5057,7 +5057,7 @@
         <v>11</v>
       </c>
       <c r="B319" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C319">
         <f t="shared" si="13"/>
@@ -5069,7 +5069,7 @@
         <v>11</v>
       </c>
       <c r="B320" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C320">
         <f t="shared" si="13"/>
@@ -5081,7 +5081,7 @@
         <v>11</v>
       </c>
       <c r="B321" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C321">
         <f t="shared" si="13"/>
@@ -5093,7 +5093,7 @@
         <v>11</v>
       </c>
       <c r="B322" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C322">
         <f t="shared" si="13"/>
@@ -5105,7 +5105,7 @@
         <v>11</v>
       </c>
       <c r="B323" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C323">
         <f t="shared" si="13"/>
@@ -5117,7 +5117,7 @@
         <v>11</v>
       </c>
       <c r="B324" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C324">
         <f t="shared" si="13"/>
@@ -5129,7 +5129,7 @@
         <v>11</v>
       </c>
       <c r="B325" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C325">
         <f t="shared" si="13"/>
@@ -5138,7 +5138,7 @@
     </row>
     <row r="328" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A328" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B328" s="6"/>
       <c r="C328" s="1">
@@ -5267,21 +5267,21 @@
     </row>
     <row r="341" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C341" s="1">
         <v>580</v>
       </c>
       <c r="J341" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B342" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C342">
         <f>C341+1</f>
@@ -5290,10 +5290,10 @@
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B343" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C343">
         <f t="shared" ref="C343:C367" si="15">C342+1</f>
@@ -5305,7 +5305,7 @@
         <v>0</v>
       </c>
       <c r="B344" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C344">
         <f t="shared" si="15"/>
@@ -5317,7 +5317,7 @@
         <v>0</v>
       </c>
       <c r="B345" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C345">
         <f t="shared" si="15"/>
@@ -5329,7 +5329,7 @@
         <v>0</v>
       </c>
       <c r="B346" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C346">
         <f t="shared" si="15"/>
@@ -5341,7 +5341,7 @@
         <v>0</v>
       </c>
       <c r="B347" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C347">
         <f t="shared" si="15"/>
@@ -5353,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="B348" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C348">
         <f t="shared" si="15"/>
@@ -5365,7 +5365,7 @@
         <v>0</v>
       </c>
       <c r="B349" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C349">
         <f t="shared" si="15"/>
@@ -5377,7 +5377,7 @@
         <v>0</v>
       </c>
       <c r="B350" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C350">
         <f t="shared" si="15"/>
@@ -5389,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="B351" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C351">
         <f t="shared" si="15"/>
@@ -5401,7 +5401,7 @@
         <v>0</v>
       </c>
       <c r="B352" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C352">
         <f t="shared" si="15"/>
@@ -5413,7 +5413,7 @@
         <v>0</v>
       </c>
       <c r="B353" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C353">
         <f t="shared" si="15"/>
@@ -5425,7 +5425,7 @@
         <v>0</v>
       </c>
       <c r="B354" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C354">
         <f t="shared" si="15"/>
@@ -5437,7 +5437,7 @@
         <v>0</v>
       </c>
       <c r="B355" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C355">
         <f t="shared" si="15"/>
@@ -5449,7 +5449,7 @@
         <v>0</v>
       </c>
       <c r="B356" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C356">
         <f t="shared" si="15"/>
@@ -5461,7 +5461,7 @@
         <v>0</v>
       </c>
       <c r="B357" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C357">
         <f t="shared" si="15"/>
@@ -5470,10 +5470,10 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B358" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C358">
         <f t="shared" si="15"/>
@@ -5482,10 +5482,10 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B359" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C359">
         <f t="shared" si="15"/>
@@ -5494,10 +5494,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B360" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C360">
         <f t="shared" si="15"/>
@@ -5509,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="B361" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C361">
         <f t="shared" si="15"/>
@@ -5521,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="B362" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C362">
         <f t="shared" si="15"/>
@@ -5533,7 +5533,7 @@
         <v>0</v>
       </c>
       <c r="B363" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C363">
         <f t="shared" si="15"/>
@@ -5545,7 +5545,7 @@
         <v>0</v>
       </c>
       <c r="B364" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C364">
         <f t="shared" si="15"/>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B365" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C365">
         <f t="shared" si="15"/>
@@ -5566,10 +5566,10 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B366" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C366">
         <f t="shared" si="15"/>
@@ -5581,7 +5581,7 @@
         <v>0</v>
       </c>
       <c r="B367" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C367">
         <f t="shared" si="15"/>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="370" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C370" s="1">
         <v>620</v>
@@ -5601,7 +5601,7 @@
         <v>87</v>
       </c>
       <c r="B371" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C371">
         <f>C370+1</f>
@@ -5613,7 +5613,7 @@
         <v>87</v>
       </c>
       <c r="B372" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C372">
         <f t="shared" ref="C372:C377" si="16">C371+1</f>
@@ -5625,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="B373" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C373">
         <f t="shared" si="16"/>
@@ -5637,7 +5637,7 @@
         <v>87</v>
       </c>
       <c r="B374" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C374">
         <f t="shared" si="16"/>
@@ -5649,7 +5649,7 @@
         <v>87</v>
       </c>
       <c r="B375" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C375">
         <f t="shared" si="16"/>
@@ -5661,7 +5661,7 @@
         <v>11</v>
       </c>
       <c r="B376" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C376">
         <f t="shared" si="16"/>
@@ -5673,7 +5673,7 @@
         <v>87</v>
       </c>
       <c r="B377" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C377">
         <f t="shared" si="16"/>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="380" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>